<commit_message>
Append Hencoder learning plan.
</commit_message>
<xml_diff>
--- a/Plan/Plan_2020_09_02.xlsx
+++ b/Plan/Plan_2020_09_02.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35">
   <si>
     <t>序号</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>每天半小时Java+Android+数据结构+操作系统+计算机网络题目练习</t>
+  </si>
+  <si>
+    <t>Hencoder</t>
+  </si>
+  <si>
+    <t>https://hencoder.com/</t>
   </si>
 </sst>
 </file>
@@ -120,10 +126,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -143,22 +149,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,21 +179,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -195,6 +187,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -203,76 +202,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,30 +299,168 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -329,145 +473,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,6 +502,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -513,9 +528,29 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,15 +570,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -558,177 +584,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -740,6 +746,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1066,7 +1075,7 @@
   <dimension ref="A2:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1126,10 +1135,10 @@
       <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>44077</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>44307</v>
       </c>
       <c r="G3" s="2"/>
@@ -1152,10 +1161,10 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>44077</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>44090</v>
       </c>
       <c r="G4" s="2"/>
@@ -1174,10 +1183,10 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>44091</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>44097</v>
       </c>
       <c r="G5" s="2"/>
@@ -1200,10 +1209,10 @@
       <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <v>44098</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>44121</v>
       </c>
       <c r="G6" s="2"/>
@@ -1228,10 +1237,10 @@
       <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <v>44122</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="2"/>
@@ -1254,10 +1263,10 @@
       <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <v>44122</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
         <v>44142</v>
       </c>
       <c r="G8" s="2"/>
@@ -1280,10 +1289,10 @@
       <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>44143</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <v>44163</v>
       </c>
       <c r="G9" s="2"/>
@@ -1306,7 +1315,7 @@
       <c r="D10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="5">
         <v>44164</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1332,10 +1341,10 @@
       <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="5">
         <v>44164</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="5">
         <v>44184</v>
       </c>
       <c r="G11" s="2"/>
@@ -1358,8 +1367,8 @@
       <c r="D12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="4">
-        <v>44184</v>
+      <c r="E12" s="5">
+        <v>44185</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>16</v>
@@ -1371,18 +1380,30 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" ht="17" spans="1:10">
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="5">
+        <v>44185</v>
+      </c>
+      <c r="F13" s="5">
+        <v>44205</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
@@ -1401,6 +1422,7 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="https://www.bilibili.com/video/BV1zE41197bw" tooltip="https://www.bilibili.com/video/BV1zE41197bw"/>
     <hyperlink ref="D8" r:id="rId2" display="https://flutterchina.club/" tooltip="https://flutterchina.club/"/>
+    <hyperlink ref="D13" r:id="rId3" display="https://hencoder.com/" tooltip="https://hencoder.com/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>